<commit_message>
added data & image
</commit_message>
<xml_diff>
--- a/Platzierungen.xlsx
+++ b/Platzierungen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dateien\Werfen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9E4957-5AE9-443F-AC0E-E746732B848B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623A15C5-33DA-411B-B614-D74BFF01BB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E380670F-4102-4798-B118-969E8673B2F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="195">
   <si>
     <t>Player 1</t>
   </si>
@@ -603,6 +603,24 @@
   </si>
   <si>
     <t>Geckabor Gangster</t>
+  </si>
+  <si>
+    <t>Lieblingswort Zaza</t>
+  </si>
+  <si>
+    <t>Normale Kartoffeln auf die Eins</t>
+  </si>
+  <si>
+    <t>Pain in the Ass (Ace)</t>
+  </si>
+  <si>
+    <t>Marwin</t>
+  </si>
+  <si>
+    <t>MFM</t>
+  </si>
+  <si>
+    <t>Pferde auf die Eins</t>
   </si>
 </sst>
 </file>
@@ -978,11 +996,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A150CB-7EA0-430C-9B05-F3D09136D85C}">
-  <dimension ref="A1:I154"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E129" sqref="E129"/>
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H159" sqref="H159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4716,6 +4734,121 @@
         <v>1</v>
       </c>
     </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>43</v>
+      </c>
+      <c r="B155" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155" t="s">
+        <v>114</v>
+      </c>
+      <c r="D155" t="s">
+        <v>189</v>
+      </c>
+      <c r="E155" s="2">
+        <v>45458</v>
+      </c>
+      <c r="F155">
+        <v>5</v>
+      </c>
+      <c r="G155">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>24</v>
+      </c>
+      <c r="B156" t="s">
+        <v>9</v>
+      </c>
+      <c r="C156" t="s">
+        <v>18</v>
+      </c>
+      <c r="D156" t="s">
+        <v>190</v>
+      </c>
+      <c r="E156" s="2">
+        <v>45458</v>
+      </c>
+      <c r="F156">
+        <v>3</v>
+      </c>
+      <c r="G156">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>70</v>
+      </c>
+      <c r="B157" t="s">
+        <v>30</v>
+      </c>
+      <c r="C157" t="s">
+        <v>77</v>
+      </c>
+      <c r="D157" t="s">
+        <v>191</v>
+      </c>
+      <c r="E157" s="2">
+        <v>45458</v>
+      </c>
+      <c r="F157">
+        <v>4</v>
+      </c>
+      <c r="G157">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>192</v>
+      </c>
+      <c r="B158" t="s">
+        <v>13</v>
+      </c>
+      <c r="C158" t="s">
+        <v>44</v>
+      </c>
+      <c r="D158" t="s">
+        <v>193</v>
+      </c>
+      <c r="E158" s="2">
+        <v>45458</v>
+      </c>
+      <c r="F158">
+        <v>2</v>
+      </c>
+      <c r="G158">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>22</v>
+      </c>
+      <c r="B159" t="s">
+        <v>87</v>
+      </c>
+      <c r="C159" t="s">
+        <v>7</v>
+      </c>
+      <c r="D159" t="s">
+        <v>194</v>
+      </c>
+      <c r="E159" s="2">
+        <v>45458</v>
+      </c>
+      <c r="F159">
+        <v>1</v>
+      </c>
+      <c r="G159">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I61">
     <sortCondition ref="E2:E61"/>

</xml_diff>

<commit_message>
inserted new data, updated todos
</commit_message>
<xml_diff>
--- a/Platzierungen.xlsx
+++ b/Platzierungen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dateien\Werfen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Werfen\werfen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623A15C5-33DA-411B-B614-D74BFF01BB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2337A24-ED38-481A-BDC0-78CAA5D31F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E380670F-4102-4798-B118-969E8673B2F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="212">
   <si>
     <t>Player 1</t>
   </si>
@@ -621,6 +621,57 @@
   </si>
   <si>
     <t>Pferde auf die Eins</t>
+  </si>
+  <si>
+    <t>Pferdewelle Stampf Stampf</t>
+  </si>
+  <si>
+    <t>Garruk Ultras</t>
+  </si>
+  <si>
+    <t>Die Prenzlauer Crew</t>
+  </si>
+  <si>
+    <t>Fleißigen Bienen Bzz Bzz</t>
+  </si>
+  <si>
+    <t>Zuckerlager voll</t>
+  </si>
+  <si>
+    <t>Alles Andere als Arbeit</t>
+  </si>
+  <si>
+    <t>DD - Dirk &amp; Dora</t>
+  </si>
+  <si>
+    <t>Team Heul doch</t>
+  </si>
+  <si>
+    <t>Die romantischen Matrosen</t>
+  </si>
+  <si>
+    <t>ZaZa Grill</t>
+  </si>
+  <si>
+    <t>Bowle Batallion</t>
+  </si>
+  <si>
+    <t>I got bit by a WIDDER</t>
+  </si>
+  <si>
+    <t>K-Hole</t>
+  </si>
+  <si>
+    <t>Leonie</t>
+  </si>
+  <si>
+    <t>Schnelle Bälle</t>
+  </si>
+  <si>
+    <t>Best LoL-Players in the room</t>
+  </si>
+  <si>
+    <t>Two Bikey Boys Go Vroom</t>
   </si>
 </sst>
 </file>
@@ -996,11 +1047,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A150CB-7EA0-430C-9B05-F3D09136D85C}">
-  <dimension ref="A1:I159"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H159" sqref="H159"/>
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4849,6 +4900,377 @@
         <v>5</v>
       </c>
     </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>22</v>
+      </c>
+      <c r="B160" t="s">
+        <v>7</v>
+      </c>
+      <c r="D160" t="s">
+        <v>195</v>
+      </c>
+      <c r="E160" s="2">
+        <v>45479</v>
+      </c>
+      <c r="F160">
+        <v>3</v>
+      </c>
+      <c r="G160">
+        <v>4</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>10</v>
+      </c>
+      <c r="B161" t="s">
+        <v>18</v>
+      </c>
+      <c r="D161" t="s">
+        <v>196</v>
+      </c>
+      <c r="E161" s="2">
+        <v>45479</v>
+      </c>
+      <c r="F161">
+        <v>1</v>
+      </c>
+      <c r="G161">
+        <v>4</v>
+      </c>
+      <c r="H161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>44</v>
+      </c>
+      <c r="B162" t="s">
+        <v>9</v>
+      </c>
+      <c r="D162" t="s">
+        <v>197</v>
+      </c>
+      <c r="E162" s="2">
+        <v>45479</v>
+      </c>
+      <c r="F162">
+        <v>3</v>
+      </c>
+      <c r="G162">
+        <v>4</v>
+      </c>
+      <c r="H162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>12</v>
+      </c>
+      <c r="B163" t="s">
+        <v>48</v>
+      </c>
+      <c r="D163" t="s">
+        <v>198</v>
+      </c>
+      <c r="E163" s="2">
+        <v>45479</v>
+      </c>
+      <c r="F163">
+        <v>3</v>
+      </c>
+      <c r="G163">
+        <v>4</v>
+      </c>
+      <c r="H163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>7</v>
+      </c>
+      <c r="B164" t="s">
+        <v>18</v>
+      </c>
+      <c r="D164" t="s">
+        <v>199</v>
+      </c>
+      <c r="E164" s="2">
+        <v>45479</v>
+      </c>
+      <c r="F164">
+        <v>1</v>
+      </c>
+      <c r="G164">
+        <v>3</v>
+      </c>
+      <c r="H164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>9</v>
+      </c>
+      <c r="B165" t="s">
+        <v>10</v>
+      </c>
+      <c r="C165" t="s">
+        <v>48</v>
+      </c>
+      <c r="D165" t="s">
+        <v>200</v>
+      </c>
+      <c r="E165" s="2">
+        <v>45479</v>
+      </c>
+      <c r="F165">
+        <v>3</v>
+      </c>
+      <c r="G165">
+        <v>3</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>22</v>
+      </c>
+      <c r="B166" t="s">
+        <v>12</v>
+      </c>
+      <c r="D166" t="s">
+        <v>201</v>
+      </c>
+      <c r="E166" s="2">
+        <v>45479</v>
+      </c>
+      <c r="F166">
+        <v>2</v>
+      </c>
+      <c r="G166">
+        <v>3</v>
+      </c>
+      <c r="H166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>12</v>
+      </c>
+      <c r="B167" t="s">
+        <v>18</v>
+      </c>
+      <c r="D167" t="s">
+        <v>202</v>
+      </c>
+      <c r="E167" s="2">
+        <v>45479</v>
+      </c>
+      <c r="F167">
+        <v>1</v>
+      </c>
+      <c r="G167">
+        <v>2</v>
+      </c>
+      <c r="H167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>7</v>
+      </c>
+      <c r="B168" t="s">
+        <v>9</v>
+      </c>
+      <c r="D168" t="s">
+        <v>203</v>
+      </c>
+      <c r="E168" s="2">
+        <v>45479</v>
+      </c>
+      <c r="F168">
+        <v>2</v>
+      </c>
+      <c r="G168">
+        <v>2</v>
+      </c>
+      <c r="H168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>22</v>
+      </c>
+      <c r="B169" t="s">
+        <v>12</v>
+      </c>
+      <c r="D169" t="s">
+        <v>204</v>
+      </c>
+      <c r="E169" s="2">
+        <v>45500</v>
+      </c>
+      <c r="F169">
+        <v>2</v>
+      </c>
+      <c r="G169">
+        <v>3</v>
+      </c>
+      <c r="H169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>7</v>
+      </c>
+      <c r="B170" t="s">
+        <v>9</v>
+      </c>
+      <c r="D170" t="s">
+        <v>206</v>
+      </c>
+      <c r="E170" s="2">
+        <v>45500</v>
+      </c>
+      <c r="F170">
+        <v>1</v>
+      </c>
+      <c r="G170">
+        <v>3</v>
+      </c>
+      <c r="H170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>18</v>
+      </c>
+      <c r="B171" t="s">
+        <v>24</v>
+      </c>
+      <c r="D171" t="s">
+        <v>205</v>
+      </c>
+      <c r="E171" s="2">
+        <v>45500</v>
+      </c>
+      <c r="F171">
+        <v>3</v>
+      </c>
+      <c r="G171">
+        <v>3</v>
+      </c>
+      <c r="H171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>9</v>
+      </c>
+      <c r="B172" t="s">
+        <v>12</v>
+      </c>
+      <c r="D172" t="s">
+        <v>207</v>
+      </c>
+      <c r="E172" s="2">
+        <v>45500</v>
+      </c>
+      <c r="F172">
+        <v>1</v>
+      </c>
+      <c r="G172">
+        <v>4</v>
+      </c>
+      <c r="H172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>18</v>
+      </c>
+      <c r="B173" t="s">
+        <v>208</v>
+      </c>
+      <c r="D173" t="s">
+        <v>209</v>
+      </c>
+      <c r="E173" s="2">
+        <v>45500</v>
+      </c>
+      <c r="F173">
+        <v>3</v>
+      </c>
+      <c r="G173">
+        <v>4</v>
+      </c>
+      <c r="H173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>22</v>
+      </c>
+      <c r="B174" t="s">
+        <v>24</v>
+      </c>
+      <c r="D174" t="s">
+        <v>210</v>
+      </c>
+      <c r="E174" s="2">
+        <v>45500</v>
+      </c>
+      <c r="F174">
+        <v>3</v>
+      </c>
+      <c r="G174">
+        <v>4</v>
+      </c>
+      <c r="H174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>30</v>
+      </c>
+      <c r="B175" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" t="s">
+        <v>211</v>
+      </c>
+      <c r="E175" s="2">
+        <v>45500</v>
+      </c>
+      <c r="F175">
+        <v>3</v>
+      </c>
+      <c r="G175">
+        <v>4</v>
+      </c>
+      <c r="H175">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I61">
     <sortCondition ref="E2:E61"/>

</xml_diff>